<commit_message>
added new apis like invoice generations and more
</commit_message>
<xml_diff>
--- a/SSC MASTER LIST.xlsx
+++ b/SSC MASTER LIST.xlsx
@@ -2448,7 +2448,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2486,6 +2486,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -2576,7 +2582,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2611,8 +2617,8 @@
     <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -2623,8 +2629,11 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2939,8 +2948,8 @@
     <col min="3" max="3" style="15" width="33.43357142857143" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="15" width="59.86214285714286" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="15" width="22.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="15" width="25.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="16" width="10.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="16" width="25.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="17" width="10.290714285714287" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="15" width="20.433571428571426" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
@@ -3256,7 +3265,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="8">
         <v>0</v>
       </c>
@@ -3282,7 +3291,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="8">
         <v>0</v>
       </c>
@@ -3308,7 +3317,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="8">
         <v>0</v>
       </c>
@@ -3334,7 +3343,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="8">
         <v>0</v>
       </c>
@@ -3360,7 +3369,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="8">
         <v>0</v>
       </c>
@@ -3386,7 +3395,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="8">
         <v>0</v>
       </c>
@@ -3412,7 +3421,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="8">
         <v>0</v>
       </c>
@@ -3438,7 +3447,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="8">
         <v>0</v>
       </c>
@@ -3464,7 +3473,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="8">
         <v>0</v>
       </c>
@@ -3490,7 +3499,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="8">
         <v>0</v>
       </c>
@@ -3516,7 +3525,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="8">
         <v>0</v>
       </c>
@@ -3542,7 +3551,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="8">
         <v>0</v>
       </c>
@@ -3568,7 +3577,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="8">
         <v>0</v>
       </c>
@@ -3594,7 +3603,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="8">
         <v>0</v>
       </c>

</xml_diff>